<commit_message>
Guardado de datos en tabla excel, muestra datos en tabla, elimino incertidumbre de gasolinera
</commit_message>
<xml_diff>
--- a/HistoricoCentro.xlsx
+++ b/HistoricoCentro.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos IDE\matlab\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos IDE\matlab\Electrolinera\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29649606-E691-4E12-BEBD-803CD4953077}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD3DD1E7-45BD-4F9D-9F35-A8EE4E0C461B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A33F091B-84F3-47EA-AED0-056C2734DF16}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{A33F091B-84F3-47EA-AED0-056C2734DF16}"/>
   </bookViews>
   <sheets>
     <sheet name="opcion1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="10">
   <si>
     <t xml:space="preserve">Hora </t>
   </si>
@@ -57,75 +57,6 @@
     <t>24 de Mayo</t>
   </si>
   <si>
-    <t>25 de Mayo</t>
-  </si>
-  <si>
-    <t>26 de Mayo</t>
-  </si>
-  <si>
-    <t>27 de Mayo</t>
-  </si>
-  <si>
-    <t>28 de Mayo</t>
-  </si>
-  <si>
-    <t>29 de Mayo</t>
-  </si>
-  <si>
-    <t>30 de Mayo</t>
-  </si>
-  <si>
-    <t>31 de Mayo</t>
-  </si>
-  <si>
-    <t>32 de Mayo</t>
-  </si>
-  <si>
-    <t>33 de Mayo</t>
-  </si>
-  <si>
-    <t>34 de Mayo</t>
-  </si>
-  <si>
-    <t>35 de Mayo</t>
-  </si>
-  <si>
-    <t>36 de Mayo</t>
-  </si>
-  <si>
-    <t>37 de Mayo</t>
-  </si>
-  <si>
-    <t>38 de Mayo</t>
-  </si>
-  <si>
-    <t>39 de Mayo</t>
-  </si>
-  <si>
-    <t>40 de Mayo</t>
-  </si>
-  <si>
-    <t>41 de Mayo</t>
-  </si>
-  <si>
-    <t>42 de Mayo</t>
-  </si>
-  <si>
-    <t>43 de Mayo</t>
-  </si>
-  <si>
-    <t>44 de Mayo</t>
-  </si>
-  <si>
-    <t>45 de Mayo</t>
-  </si>
-  <si>
-    <t>46 de Mayo</t>
-  </si>
-  <si>
-    <t>47 de Mayo</t>
-  </si>
-  <si>
     <t xml:space="preserve">Borrero </t>
   </si>
 </sst>
@@ -135,8 +66,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="168" formatCode="h:mm:ss;@"/>
-    <numFmt numFmtId="169" formatCode="[$-409]h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="165" formatCode="h:mm:ss;@"/>
+    <numFmt numFmtId="166" formatCode="[$-409]h:mm\ AM/PM;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -185,8 +116,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,7 +434,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DEFE987-656B-4D68-AD41-C163EF774C17}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -543,7 +474,7 @@
       </c>
       <c r="D2">
         <f ca="1">RANDBETWEEN(100,500)</f>
-        <v>173</v>
+        <v>252</v>
       </c>
       <c r="E2">
         <v>34</v>
@@ -561,7 +492,7 @@
       </c>
       <c r="D3">
         <f ca="1">RANDBETWEEN(100,500)</f>
-        <v>387</v>
+        <v>363</v>
       </c>
       <c r="E3">
         <v>34</v>
@@ -579,7 +510,7 @@
       </c>
       <c r="D4">
         <f t="shared" ref="D4:D25" ca="1" si="0">RANDBETWEEN(100,500)</f>
-        <v>318</v>
+        <v>267</v>
       </c>
       <c r="E4">
         <v>34</v>
@@ -597,7 +528,7 @@
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>486</v>
+        <v>470</v>
       </c>
       <c r="E5">
         <v>34</v>
@@ -615,7 +546,7 @@
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>207</v>
+        <v>292</v>
       </c>
       <c r="E6">
         <v>34</v>
@@ -633,7 +564,7 @@
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>175</v>
+        <v>395</v>
       </c>
       <c r="E7">
         <v>34</v>
@@ -651,7 +582,7 @@
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>473</v>
+        <v>167</v>
       </c>
       <c r="E8">
         <v>34</v>
@@ -669,7 +600,7 @@
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>466</v>
+        <v>185</v>
       </c>
       <c r="E9">
         <v>34</v>
@@ -687,7 +618,7 @@
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>330</v>
+        <v>340</v>
       </c>
       <c r="E10">
         <v>34</v>
@@ -705,7 +636,7 @@
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="0"/>
-        <v>109</v>
+        <v>152</v>
       </c>
       <c r="E11">
         <v>34</v>
@@ -723,7 +654,7 @@
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="0"/>
-        <v>253</v>
+        <v>410</v>
       </c>
       <c r="E12">
         <v>34</v>
@@ -741,7 +672,7 @@
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="0"/>
-        <v>104</v>
+        <v>482</v>
       </c>
       <c r="E13">
         <v>34</v>
@@ -759,7 +690,7 @@
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="0"/>
-        <v>405</v>
+        <v>390</v>
       </c>
       <c r="E14">
         <v>34</v>
@@ -777,7 +708,7 @@
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
-        <v>479</v>
+        <v>459</v>
       </c>
       <c r="E15">
         <v>34</v>
@@ -795,7 +726,7 @@
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="0"/>
-        <v>453</v>
+        <v>476</v>
       </c>
       <c r="E16">
         <v>34</v>
@@ -813,7 +744,7 @@
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="0"/>
-        <v>403</v>
+        <v>204</v>
       </c>
       <c r="E17">
         <v>34</v>
@@ -831,7 +762,7 @@
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="0"/>
-        <v>170</v>
+        <v>228</v>
       </c>
       <c r="E18">
         <v>34</v>
@@ -849,7 +780,7 @@
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="0"/>
-        <v>215</v>
+        <v>328</v>
       </c>
       <c r="E19">
         <v>34</v>
@@ -867,7 +798,7 @@
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="0"/>
-        <v>351</v>
+        <v>276</v>
       </c>
       <c r="E20">
         <v>34</v>
@@ -885,7 +816,7 @@
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="0"/>
-        <v>355</v>
+        <v>105</v>
       </c>
       <c r="E21">
         <v>34</v>
@@ -903,7 +834,7 @@
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="0"/>
-        <v>347</v>
+        <v>268</v>
       </c>
       <c r="E22">
         <v>34</v>
@@ -921,7 +852,7 @@
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="0"/>
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="E23">
         <v>34</v>
@@ -939,7 +870,7 @@
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="0"/>
-        <v>190</v>
+        <v>235</v>
       </c>
       <c r="E24">
         <v>34</v>
@@ -957,7 +888,7 @@
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="0"/>
-        <v>463</v>
+        <v>473</v>
       </c>
       <c r="E25">
         <v>34</v>
@@ -1011,7 +942,7 @@
       </c>
       <c r="D2">
         <f ca="1">RANDBETWEEN(100,500)</f>
-        <v>249</v>
+        <v>178</v>
       </c>
       <c r="E2">
         <v>34</v>
@@ -1029,7 +960,7 @@
       </c>
       <c r="D3">
         <f ca="1">RANDBETWEEN(100,500)</f>
-        <v>324</v>
+        <v>221</v>
       </c>
       <c r="E3">
         <v>34</v>
@@ -1047,7 +978,7 @@
       </c>
       <c r="D4">
         <f t="shared" ref="D4:D25" ca="1" si="0">RANDBETWEEN(100,500)</f>
-        <v>177</v>
+        <v>417</v>
       </c>
       <c r="E4">
         <v>34</v>
@@ -1065,7 +996,7 @@
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>196</v>
+        <v>300</v>
       </c>
       <c r="E5">
         <v>34</v>
@@ -1083,7 +1014,7 @@
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>440</v>
+        <v>157</v>
       </c>
       <c r="E6">
         <v>34</v>
@@ -1101,7 +1032,7 @@
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>232</v>
+        <v>385</v>
       </c>
       <c r="E7">
         <v>34</v>
@@ -1119,7 +1050,7 @@
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>182</v>
+        <v>144</v>
       </c>
       <c r="E8">
         <v>34</v>
@@ -1137,7 +1068,7 @@
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>393</v>
+        <v>349</v>
       </c>
       <c r="E9">
         <v>34</v>
@@ -1155,7 +1086,7 @@
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>225</v>
+        <v>491</v>
       </c>
       <c r="E10">
         <v>34</v>
@@ -1173,7 +1104,7 @@
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="0"/>
-        <v>106</v>
+        <v>184</v>
       </c>
       <c r="E11">
         <v>34</v>
@@ -1191,7 +1122,7 @@
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="0"/>
-        <v>382</v>
+        <v>131</v>
       </c>
       <c r="E12">
         <v>34</v>
@@ -1209,7 +1140,7 @@
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="0"/>
-        <v>360</v>
+        <v>197</v>
       </c>
       <c r="E13">
         <v>34</v>
@@ -1227,7 +1158,7 @@
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="0"/>
-        <v>455</v>
+        <v>493</v>
       </c>
       <c r="E14">
         <v>34</v>
@@ -1245,7 +1176,7 @@
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
-        <v>257</v>
+        <v>277</v>
       </c>
       <c r="E15">
         <v>34</v>
@@ -1263,7 +1194,7 @@
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="0"/>
-        <v>165</v>
+        <v>258</v>
       </c>
       <c r="E16">
         <v>34</v>
@@ -1281,7 +1212,7 @@
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="0"/>
-        <v>364</v>
+        <v>470</v>
       </c>
       <c r="E17">
         <v>34</v>
@@ -1299,7 +1230,7 @@
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="0"/>
-        <v>437</v>
+        <v>320</v>
       </c>
       <c r="E18">
         <v>34</v>
@@ -1317,7 +1248,7 @@
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="0"/>
-        <v>212</v>
+        <v>188</v>
       </c>
       <c r="E19">
         <v>34</v>
@@ -1335,7 +1266,7 @@
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="0"/>
-        <v>134</v>
+        <v>174</v>
       </c>
       <c r="E20">
         <v>34</v>
@@ -1353,7 +1284,7 @@
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="0"/>
-        <v>363</v>
+        <v>252</v>
       </c>
       <c r="E21">
         <v>34</v>
@@ -1371,7 +1302,7 @@
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="0"/>
-        <v>169</v>
+        <v>230</v>
       </c>
       <c r="E22">
         <v>34</v>
@@ -1389,7 +1320,7 @@
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="0"/>
-        <v>424</v>
+        <v>469</v>
       </c>
       <c r="E23">
         <v>34</v>
@@ -1407,7 +1338,7 @@
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="0"/>
-        <v>319</v>
+        <v>423</v>
       </c>
       <c r="E24">
         <v>34</v>
@@ -1425,7 +1356,7 @@
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="0"/>
-        <v>372</v>
+        <v>380</v>
       </c>
       <c r="E25">
         <v>34</v>
@@ -1440,8 +1371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C35CD5A5-1F47-48CC-962F-FC7AEB0D7686}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1475,7 +1406,7 @@
       </c>
       <c r="D2">
         <f ca="1">RANDBETWEEN(100,500)</f>
-        <v>267</v>
+        <v>106</v>
       </c>
       <c r="E2">
         <v>34</v>
@@ -1489,11 +1420,11 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3">
         <f ca="1">RANDBETWEEN(100,500)</f>
-        <v>428</v>
+        <v>134</v>
       </c>
       <c r="E3">
         <v>34</v>
@@ -1507,11 +1438,11 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4:D25" ca="1" si="0">RANDBETWEEN(100,500)</f>
-        <v>291</v>
+        <v>122</v>
       </c>
       <c r="E4">
         <v>34</v>
@@ -1525,11 +1456,11 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>360</v>
+        <v>123</v>
       </c>
       <c r="E5">
         <v>34</v>
@@ -1543,11 +1474,11 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>475</v>
+        <v>496</v>
       </c>
       <c r="E6">
         <v>34</v>
@@ -1561,11 +1492,11 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>267</v>
+        <v>381</v>
       </c>
       <c r="E7">
         <v>34</v>
@@ -1579,11 +1510,11 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>393</v>
+        <v>365</v>
       </c>
       <c r="E8">
         <v>34</v>
@@ -1597,11 +1528,11 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>214</v>
+        <v>425</v>
       </c>
       <c r="E9">
         <v>34</v>
@@ -1615,11 +1546,11 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>253</v>
+        <v>117</v>
       </c>
       <c r="E10">
         <v>34</v>
@@ -1633,11 +1564,11 @@
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="0"/>
-        <v>190</v>
+        <v>408</v>
       </c>
       <c r="E11">
         <v>34</v>
@@ -1651,11 +1582,11 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="0"/>
-        <v>496</v>
+        <v>241</v>
       </c>
       <c r="E12">
         <v>34</v>
@@ -1669,11 +1600,11 @@
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="0"/>
-        <v>218</v>
+        <v>329</v>
       </c>
       <c r="E13">
         <v>34</v>
@@ -1687,11 +1618,11 @@
         <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="0"/>
-        <v>106</v>
+        <v>248</v>
       </c>
       <c r="E14">
         <v>34</v>
@@ -1705,11 +1636,11 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
-        <v>167</v>
+        <v>139</v>
       </c>
       <c r="E15">
         <v>34</v>
@@ -1723,11 +1654,11 @@
         <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="0"/>
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E16">
         <v>34</v>
@@ -1741,11 +1672,11 @@
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="0"/>
-        <v>108</v>
+        <v>271</v>
       </c>
       <c r="E17">
         <v>34</v>
@@ -1759,11 +1690,11 @@
         <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="0"/>
-        <v>353</v>
+        <v>427</v>
       </c>
       <c r="E18">
         <v>34</v>
@@ -1777,11 +1708,11 @@
         <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="0"/>
-        <v>193</v>
+        <v>428</v>
       </c>
       <c r="E19">
         <v>34</v>
@@ -1795,11 +1726,11 @@
         <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="0"/>
-        <v>277</v>
+        <v>203</v>
       </c>
       <c r="E20">
         <v>34</v>
@@ -1813,11 +1744,11 @@
         <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="0"/>
-        <v>438</v>
+        <v>406</v>
       </c>
       <c r="E21">
         <v>34</v>
@@ -1831,11 +1762,11 @@
         <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="0"/>
-        <v>357</v>
+        <v>127</v>
       </c>
       <c r="E22">
         <v>34</v>
@@ -1849,11 +1780,11 @@
         <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="0"/>
-        <v>459</v>
+        <v>290</v>
       </c>
       <c r="E23">
         <v>34</v>
@@ -1867,11 +1798,11 @@
         <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="0"/>
-        <v>332</v>
+        <v>290</v>
       </c>
       <c r="E24">
         <v>34</v>
@@ -1885,11 +1816,11 @@
         <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="0"/>
-        <v>373</v>
+        <v>425</v>
       </c>
       <c r="E25">
         <v>34</v>
@@ -1936,11 +1867,11 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="D2">
         <f ca="1">RANDBETWEEN(100,500)</f>
-        <v>362</v>
+        <v>172</v>
       </c>
       <c r="E2">
         <v>34</v>
@@ -1954,11 +1885,11 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="D3">
         <f ca="1">RANDBETWEEN(100,500)</f>
-        <v>298</v>
+        <v>218</v>
       </c>
       <c r="E3">
         <v>34</v>
@@ -1972,11 +1903,11 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4:D25" ca="1" si="0">RANDBETWEEN(100,500)</f>
-        <v>467</v>
+        <v>459</v>
       </c>
       <c r="E4">
         <v>34</v>
@@ -1990,11 +1921,11 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>426</v>
+        <v>352</v>
       </c>
       <c r="E5">
         <v>34</v>
@@ -2008,11 +1939,11 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>179</v>
+        <v>163</v>
       </c>
       <c r="E6">
         <v>34</v>
@@ -2026,11 +1957,11 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>460</v>
+        <v>484</v>
       </c>
       <c r="E7">
         <v>34</v>
@@ -2044,11 +1975,11 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>457</v>
+        <v>144</v>
       </c>
       <c r="E8">
         <v>34</v>
@@ -2062,11 +1993,11 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>176</v>
+        <v>155</v>
       </c>
       <c r="E9">
         <v>34</v>
@@ -2080,11 +2011,11 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>279</v>
+        <v>239</v>
       </c>
       <c r="E10">
         <v>34</v>
@@ -2098,11 +2029,11 @@
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="0"/>
-        <v>213</v>
+        <v>192</v>
       </c>
       <c r="E11">
         <v>34</v>
@@ -2116,11 +2047,11 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="0"/>
-        <v>324</v>
+        <v>275</v>
       </c>
       <c r="E12">
         <v>34</v>
@@ -2134,11 +2065,11 @@
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="0"/>
-        <v>403</v>
+        <v>321</v>
       </c>
       <c r="E13">
         <v>34</v>
@@ -2152,11 +2083,11 @@
         <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="0"/>
-        <v>388</v>
+        <v>359</v>
       </c>
       <c r="E14">
         <v>34</v>
@@ -2170,11 +2101,11 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
-        <v>105</v>
+        <v>311</v>
       </c>
       <c r="E15">
         <v>34</v>
@@ -2188,11 +2119,11 @@
         <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="0"/>
-        <v>383</v>
+        <v>358</v>
       </c>
       <c r="E16">
         <v>34</v>
@@ -2206,11 +2137,11 @@
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="0"/>
-        <v>445</v>
+        <v>415</v>
       </c>
       <c r="E17">
         <v>34</v>
@@ -2224,11 +2155,11 @@
         <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="0"/>
-        <v>126</v>
+        <v>447</v>
       </c>
       <c r="E18">
         <v>34</v>
@@ -2242,11 +2173,11 @@
         <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="0"/>
-        <v>263</v>
+        <v>248</v>
       </c>
       <c r="E19">
         <v>34</v>
@@ -2260,11 +2191,11 @@
         <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="0"/>
-        <v>184</v>
+        <v>202</v>
       </c>
       <c r="E20">
         <v>34</v>
@@ -2278,11 +2209,11 @@
         <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="0"/>
-        <v>370</v>
+        <v>350</v>
       </c>
       <c r="E21">
         <v>34</v>
@@ -2296,11 +2227,11 @@
         <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="0"/>
-        <v>229</v>
+        <v>254</v>
       </c>
       <c r="E22">
         <v>34</v>
@@ -2315,11 +2246,11 @@
         <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="0"/>
-        <v>414</v>
+        <v>362</v>
       </c>
       <c r="E23">
         <v>34</v>
@@ -2333,11 +2264,11 @@
         <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="0"/>
-        <v>432</v>
+        <v>204</v>
       </c>
       <c r="E24">
         <v>34</v>
@@ -2351,11 +2282,11 @@
         <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="0"/>
-        <v>322</v>
+        <v>209</v>
       </c>
       <c r="E25">
         <v>34</v>

</xml_diff>